<commit_message>
Version 1.0.0 completed the pages and Test cases
</commit_message>
<xml_diff>
--- a/data/EditLead.xlsx
+++ b/data/EditLead.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TestLeaf\wTestLeafSpace\POM\datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TestLeaf\Code\framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6025015-D52D-49B8-9E9D-0C75342F5A51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444AC0B7-8983-4C27-8D0A-E5B1CBF1EFBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,13 +51,13 @@
     <t>crmsfa</t>
   </si>
   <si>
-    <t>demosalesCSR</t>
-  </si>
-  <si>
     <t>Update Company Name</t>
   </si>
   <si>
     <t>Amazon</t>
+  </si>
+  <si>
+    <t>DemoCSR</t>
   </si>
 </sst>
 </file>
@@ -395,7 +395,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +417,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -436,7 +436,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -445,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>